<commit_message>
Diverse ändringar av felaktigheter
</commit_message>
<xml_diff>
--- a/Indata/sjukpenningtal.xlsx
+++ b/Indata/sjukpenningtal.xlsx
@@ -47,7 +47,7 @@
     <t xml:space="preserve">2024</t>
   </si>
   <si>
-    <t xml:space="preserve">10</t>
+    <t xml:space="preserve">11</t>
   </si>
   <si>
     <t xml:space="preserve">00 Riket</t>
@@ -65,7 +65,7 @@
     <t xml:space="preserve">Riket</t>
   </si>
   <si>
-    <t xml:space="preserve">oktober</t>
+    <t xml:space="preserve">november</t>
   </si>
   <si>
     <t xml:space="preserve">Kvinnor</t>
@@ -500,7 +500,7 @@
         <v>14</v>
       </c>
       <c r="G2" t="n">
-        <v>10.4</v>
+        <v>10.5</v>
       </c>
       <c r="H2" t="s">
         <v>15</v>
@@ -532,7 +532,7 @@
         <v>18</v>
       </c>
       <c r="G3" t="n">
-        <v>13.6</v>
+        <v>13.7</v>
       </c>
       <c r="H3" t="s">
         <v>15</v>
@@ -788,7 +788,7 @@
         <v>14</v>
       </c>
       <c r="G11" t="n">
-        <v>10.7</v>
+        <v>10.8</v>
       </c>
       <c r="H11" t="s">
         <v>15</v>
@@ -820,7 +820,7 @@
         <v>18</v>
       </c>
       <c r="G12" t="n">
-        <v>14.3</v>
+        <v>14.5</v>
       </c>
       <c r="H12" t="s">
         <v>15</v>
@@ -884,7 +884,7 @@
         <v>14</v>
       </c>
       <c r="G14" t="n">
-        <v>11.3</v>
+        <v>11.4</v>
       </c>
       <c r="H14" t="s">
         <v>15</v>
@@ -916,7 +916,7 @@
         <v>18</v>
       </c>
       <c r="G15" t="n">
-        <v>15.6</v>
+        <v>15.7</v>
       </c>
       <c r="H15" t="s">
         <v>15</v>
@@ -980,7 +980,7 @@
         <v>14</v>
       </c>
       <c r="G17" t="n">
-        <v>14.6</v>
+        <v>14.7</v>
       </c>
       <c r="H17" t="s">
         <v>15</v>
@@ -1012,7 +1012,7 @@
         <v>18</v>
       </c>
       <c r="G18" t="n">
-        <v>18.9</v>
+        <v>19.1</v>
       </c>
       <c r="H18" t="s">
         <v>15</v>
@@ -1076,7 +1076,7 @@
         <v>14</v>
       </c>
       <c r="G20" t="n">
-        <v>17.9</v>
+        <v>18</v>
       </c>
       <c r="H20" t="s">
         <v>15</v>
@@ -1108,7 +1108,7 @@
         <v>18</v>
       </c>
       <c r="G21" t="n">
-        <v>20.9</v>
+        <v>21.1</v>
       </c>
       <c r="H21" t="s">
         <v>15</v>
@@ -1140,7 +1140,7 @@
         <v>19</v>
       </c>
       <c r="G22" t="n">
-        <v>14.9</v>
+        <v>15</v>
       </c>
       <c r="H22" t="s">
         <v>15</v>
@@ -1172,7 +1172,7 @@
         <v>14</v>
       </c>
       <c r="G23" t="n">
-        <v>13</v>
+        <v>13.2</v>
       </c>
       <c r="H23" t="s">
         <v>27</v>
@@ -1204,7 +1204,7 @@
         <v>18</v>
       </c>
       <c r="G24" t="n">
-        <v>17.8</v>
+        <v>18</v>
       </c>
       <c r="H24" t="s">
         <v>27</v>
@@ -1332,7 +1332,7 @@
         <v>19</v>
       </c>
       <c r="G28" t="n">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="H28" t="s">
         <v>27</v>
@@ -1364,7 +1364,7 @@
         <v>14</v>
       </c>
       <c r="G29" t="n">
-        <v>6</v>
+        <v>6.1</v>
       </c>
       <c r="H29" t="s">
         <v>27</v>
@@ -1396,7 +1396,7 @@
         <v>18</v>
       </c>
       <c r="G30" t="n">
-        <v>8.7</v>
+        <v>8.8</v>
       </c>
       <c r="H30" t="s">
         <v>27</v>
@@ -1428,7 +1428,7 @@
         <v>19</v>
       </c>
       <c r="G31" t="n">
-        <v>3.5</v>
+        <v>3.6</v>
       </c>
       <c r="H31" t="s">
         <v>27</v>
@@ -1460,7 +1460,7 @@
         <v>14</v>
       </c>
       <c r="G32" t="n">
-        <v>14.5</v>
+        <v>14.8</v>
       </c>
       <c r="H32" t="s">
         <v>27</v>
@@ -1492,7 +1492,7 @@
         <v>18</v>
       </c>
       <c r="G33" t="n">
-        <v>20.6</v>
+        <v>21.1</v>
       </c>
       <c r="H33" t="s">
         <v>27</v>
@@ -1524,7 +1524,7 @@
         <v>19</v>
       </c>
       <c r="G34" t="n">
-        <v>8.7</v>
+        <v>8.8</v>
       </c>
       <c r="H34" t="s">
         <v>27</v>
@@ -1556,7 +1556,7 @@
         <v>14</v>
       </c>
       <c r="G35" t="n">
-        <v>15.1</v>
+        <v>15.4</v>
       </c>
       <c r="H35" t="s">
         <v>27</v>
@@ -1588,7 +1588,7 @@
         <v>18</v>
       </c>
       <c r="G36" t="n">
-        <v>21.2</v>
+        <v>21.5</v>
       </c>
       <c r="H36" t="s">
         <v>27</v>
@@ -1620,7 +1620,7 @@
         <v>19</v>
       </c>
       <c r="G37" t="n">
-        <v>9.2</v>
+        <v>9.4</v>
       </c>
       <c r="H37" t="s">
         <v>27</v>
@@ -1652,7 +1652,7 @@
         <v>14</v>
       </c>
       <c r="G38" t="n">
-        <v>17.4</v>
+        <v>17.5</v>
       </c>
       <c r="H38" t="s">
         <v>27</v>
@@ -1684,7 +1684,7 @@
         <v>18</v>
       </c>
       <c r="G39" t="n">
-        <v>22.8</v>
+        <v>23.1</v>
       </c>
       <c r="H39" t="s">
         <v>27</v>
@@ -1716,7 +1716,7 @@
         <v>19</v>
       </c>
       <c r="G40" t="n">
-        <v>12.3</v>
+        <v>12.2</v>
       </c>
       <c r="H40" t="s">
         <v>27</v>
@@ -1748,7 +1748,7 @@
         <v>14</v>
       </c>
       <c r="G41" t="n">
-        <v>18.9</v>
+        <v>19</v>
       </c>
       <c r="H41" t="s">
         <v>27</v>
@@ -1780,7 +1780,7 @@
         <v>18</v>
       </c>
       <c r="G42" t="n">
-        <v>22.9</v>
+        <v>23.2</v>
       </c>
       <c r="H42" t="s">
         <v>27</v>
@@ -1844,7 +1844,7 @@
         <v>14</v>
       </c>
       <c r="G44" t="n">
-        <v>12.6</v>
+        <v>12.7</v>
       </c>
       <c r="H44" t="s">
         <v>30</v>
@@ -1876,7 +1876,7 @@
         <v>18</v>
       </c>
       <c r="G45" t="n">
-        <v>16.8</v>
+        <v>17</v>
       </c>
       <c r="H45" t="s">
         <v>30</v>
@@ -2100,7 +2100,7 @@
         <v>19</v>
       </c>
       <c r="G52" t="n">
-        <v>5</v>
+        <v>4.9</v>
       </c>
       <c r="H52" t="s">
         <v>30</v>
@@ -2164,7 +2164,7 @@
         <v>18</v>
       </c>
       <c r="G54" t="n">
-        <v>18.7</v>
+        <v>18.8</v>
       </c>
       <c r="H54" t="s">
         <v>30</v>
@@ -2228,7 +2228,7 @@
         <v>14</v>
       </c>
       <c r="G56" t="n">
-        <v>13.6</v>
+        <v>13.7</v>
       </c>
       <c r="H56" t="s">
         <v>30</v>
@@ -2260,7 +2260,7 @@
         <v>18</v>
       </c>
       <c r="G57" t="n">
-        <v>19</v>
+        <v>19.2</v>
       </c>
       <c r="H57" t="s">
         <v>30</v>
@@ -2324,7 +2324,7 @@
         <v>14</v>
       </c>
       <c r="G59" t="n">
-        <v>15.9</v>
+        <v>16.1</v>
       </c>
       <c r="H59" t="s">
         <v>30</v>
@@ -2356,7 +2356,7 @@
         <v>18</v>
       </c>
       <c r="G60" t="n">
-        <v>21</v>
+        <v>21.4</v>
       </c>
       <c r="H60" t="s">
         <v>30</v>
@@ -2420,7 +2420,7 @@
         <v>14</v>
       </c>
       <c r="G62" t="n">
-        <v>18.5</v>
+        <v>18.6</v>
       </c>
       <c r="H62" t="s">
         <v>30</v>
@@ -2516,7 +2516,7 @@
         <v>14</v>
       </c>
       <c r="G65" t="n">
-        <v>12.9</v>
+        <v>13</v>
       </c>
       <c r="H65" t="s">
         <v>33</v>
@@ -2548,7 +2548,7 @@
         <v>18</v>
       </c>
       <c r="G66" t="n">
-        <v>17</v>
+        <v>17.2</v>
       </c>
       <c r="H66" t="s">
         <v>33</v>
@@ -2580,7 +2580,7 @@
         <v>19</v>
       </c>
       <c r="G67" t="n">
-        <v>9</v>
+        <v>9.1</v>
       </c>
       <c r="H67" t="s">
         <v>33</v>
@@ -2740,7 +2740,7 @@
         <v>18</v>
       </c>
       <c r="G72" t="n">
-        <v>7.3</v>
+        <v>7.4</v>
       </c>
       <c r="H72" t="s">
         <v>33</v>
@@ -2772,7 +2772,7 @@
         <v>19</v>
       </c>
       <c r="G73" t="n">
-        <v>4.2</v>
+        <v>4.1</v>
       </c>
       <c r="H73" t="s">
         <v>33</v>
@@ -2804,7 +2804,7 @@
         <v>14</v>
       </c>
       <c r="G74" t="n">
-        <v>13.6</v>
+        <v>13.8</v>
       </c>
       <c r="H74" t="s">
         <v>33</v>
@@ -2836,7 +2836,7 @@
         <v>18</v>
       </c>
       <c r="G75" t="n">
-        <v>18.6</v>
+        <v>18.9</v>
       </c>
       <c r="H75" t="s">
         <v>33</v>
@@ -2900,7 +2900,7 @@
         <v>14</v>
       </c>
       <c r="G77" t="n">
-        <v>14.2</v>
+        <v>14.4</v>
       </c>
       <c r="H77" t="s">
         <v>33</v>
@@ -2932,7 +2932,7 @@
         <v>18</v>
       </c>
       <c r="G78" t="n">
-        <v>19.3</v>
+        <v>19.6</v>
       </c>
       <c r="H78" t="s">
         <v>33</v>
@@ -2964,7 +2964,7 @@
         <v>19</v>
       </c>
       <c r="G79" t="n">
-        <v>9.1</v>
+        <v>9.2</v>
       </c>
       <c r="H79" t="s">
         <v>33</v>
@@ -2996,7 +2996,7 @@
         <v>14</v>
       </c>
       <c r="G80" t="n">
-        <v>17.7</v>
+        <v>17.8</v>
       </c>
       <c r="H80" t="s">
         <v>33</v>
@@ -3028,7 +3028,7 @@
         <v>18</v>
       </c>
       <c r="G81" t="n">
-        <v>23.3</v>
+        <v>23.5</v>
       </c>
       <c r="H81" t="s">
         <v>33</v>
@@ -3060,7 +3060,7 @@
         <v>19</v>
       </c>
       <c r="G82" t="n">
-        <v>12.3</v>
+        <v>12.5</v>
       </c>
       <c r="H82" t="s">
         <v>33</v>
@@ -3092,7 +3092,7 @@
         <v>14</v>
       </c>
       <c r="G83" t="n">
-        <v>20.2</v>
+        <v>20.5</v>
       </c>
       <c r="H83" t="s">
         <v>33</v>
@@ -3124,7 +3124,7 @@
         <v>18</v>
       </c>
       <c r="G84" t="n">
-        <v>23.4</v>
+        <v>23.9</v>
       </c>
       <c r="H84" t="s">
         <v>33</v>
@@ -3156,7 +3156,7 @@
         <v>19</v>
       </c>
       <c r="G85" t="n">
-        <v>17.1</v>
+        <v>17.3</v>
       </c>
       <c r="H85" t="s">
         <v>33</v>

</xml_diff>